<commit_message>
[RF GEN] path review - company work
</commit_message>
<xml_diff>
--- a/1_Schematic/Build V1.0/RF-GEN-Path tune data_20200127.xlsx
+++ b/1_Schematic/Build V1.0/RF-GEN-Path tune data_20200127.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Backup\Plasma_RF_Generator\1_Schematic\Build V1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{436C0858-3A64-4585-9C3F-0344B9B83116}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F9AAC60-8233-4C15-99C2-AED19E0FEE35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="LT1210" sheetId="1" r:id="rId1"/>
+    <sheet name="Changed list" sheetId="3" r:id="rId1"/>
     <sheet name="AD8051" sheetId="2" r:id="rId2"/>
+    <sheet name="AD8051 (2)" sheetId="4" r:id="rId3"/>
+    <sheet name="LT1210" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="69">
   <si>
     <t>Origin</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -293,7 +295,88 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>R36</t>
+    <t>No</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sheet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reference</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Before</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>After</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Remark</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PCB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Load</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P[mW]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Irms[mA]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>R36[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>Ω</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>]</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2/1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.2uF</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -301,10 +384,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="178" formatCode="0.0"/>
+  <numFmts count="3">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="0.0"/>
+    <numFmt numFmtId="180" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -349,8 +434,15 @@
       <name val="맑은 고딕"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -369,8 +461,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="16">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -597,52 +695,94 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
@@ -650,9 +790,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="0" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -666,18 +806,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -685,14 +819,119 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="41" fontId="0" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="쉼표 [0]" xfId="1" builtinId="6"/>
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -970,11 +1209,1340 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1583C18A-FB4D-440C-9D20-9263D54605E0}">
+  <dimension ref="B2:J14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F18" sqref="F18:F19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="4.5" customWidth="1"/>
+    <col min="2" max="2" width="3.8984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.8984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.8984375" customWidth="1"/>
+    <col min="5" max="5" width="6.19921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5" customWidth="1"/>
+    <col min="7" max="8" width="25.5" customWidth="1"/>
+    <col min="9" max="9" width="45.296875" customWidth="1"/>
+    <col min="10" max="10" width="25.296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:10" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="3" spans="2:10" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B3" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="45" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="45" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" s="45" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" s="45" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" s="45" t="s">
+        <v>57</v>
+      </c>
+      <c r="H3" s="45" t="s">
+        <v>58</v>
+      </c>
+      <c r="I3" s="46" t="s">
+        <v>59</v>
+      </c>
+      <c r="J3" s="47" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="48">
+        <v>1</v>
+      </c>
+      <c r="C4" s="49"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="51"/>
+      <c r="J4" s="52"/>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B5" s="53">
+        <v>2</v>
+      </c>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="55"/>
+      <c r="G5" s="55"/>
+      <c r="H5" s="55"/>
+      <c r="I5" s="56"/>
+      <c r="J5" s="57"/>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B6" s="53">
+        <v>3</v>
+      </c>
+      <c r="C6" s="54"/>
+      <c r="D6" s="54"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="55"/>
+      <c r="G6" s="55"/>
+      <c r="H6" s="55"/>
+      <c r="I6" s="56"/>
+      <c r="J6" s="57"/>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B7" s="53">
+        <v>4</v>
+      </c>
+      <c r="C7" s="54"/>
+      <c r="D7" s="54"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="55"/>
+      <c r="G7" s="55"/>
+      <c r="H7" s="55"/>
+      <c r="I7" s="56"/>
+      <c r="J7" s="57"/>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B8" s="53">
+        <v>5</v>
+      </c>
+      <c r="C8" s="54"/>
+      <c r="D8" s="54"/>
+      <c r="E8" s="55"/>
+      <c r="F8" s="55"/>
+      <c r="G8" s="55"/>
+      <c r="H8" s="55"/>
+      <c r="I8" s="56"/>
+      <c r="J8" s="57"/>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B9" s="53">
+        <v>6</v>
+      </c>
+      <c r="C9" s="54"/>
+      <c r="D9" s="54"/>
+      <c r="E9" s="55"/>
+      <c r="F9" s="55"/>
+      <c r="G9" s="55"/>
+      <c r="H9" s="55"/>
+      <c r="I9" s="56"/>
+      <c r="J9" s="57"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B10" s="53">
+        <v>7</v>
+      </c>
+      <c r="C10" s="54"/>
+      <c r="D10" s="54"/>
+      <c r="E10" s="55"/>
+      <c r="F10" s="55"/>
+      <c r="G10" s="55"/>
+      <c r="H10" s="55"/>
+      <c r="I10" s="56"/>
+      <c r="J10" s="57"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B11" s="53">
+        <v>8</v>
+      </c>
+      <c r="C11" s="54"/>
+      <c r="D11" s="54"/>
+      <c r="E11" s="55"/>
+      <c r="F11" s="55"/>
+      <c r="G11" s="55"/>
+      <c r="H11" s="58"/>
+      <c r="I11" s="63"/>
+      <c r="J11" s="57"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B12" s="53">
+        <v>9</v>
+      </c>
+      <c r="C12" s="54"/>
+      <c r="D12" s="54"/>
+      <c r="E12" s="55"/>
+      <c r="F12" s="55"/>
+      <c r="G12" s="55"/>
+      <c r="H12" s="58"/>
+      <c r="I12" s="63"/>
+      <c r="J12" s="57"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B13" s="53">
+        <v>10</v>
+      </c>
+      <c r="C13" s="54"/>
+      <c r="D13" s="54"/>
+      <c r="E13" s="56"/>
+      <c r="F13" s="55"/>
+      <c r="G13" s="55"/>
+      <c r="H13" s="55"/>
+      <c r="I13" s="58"/>
+      <c r="J13" s="57"/>
+    </row>
+    <row r="14" spans="2:10" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B14" s="53">
+        <v>11</v>
+      </c>
+      <c r="C14" s="59"/>
+      <c r="D14" s="59"/>
+      <c r="E14" s="64"/>
+      <c r="F14" s="60"/>
+      <c r="G14" s="60"/>
+      <c r="H14" s="60"/>
+      <c r="I14" s="61"/>
+      <c r="J14" s="62"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E953C177-0DFA-4874-B49C-BF9F6EC2E1F7}">
+  <dimension ref="B3:W13"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="2.3984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:23" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="4" spans="2:23" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B4" s="26"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="68" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="68"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
+      <c r="H4" s="67"/>
+      <c r="I4" s="67"/>
+      <c r="J4" s="67"/>
+      <c r="K4" s="67"/>
+      <c r="M4" s="67"/>
+      <c r="N4" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="O4" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="P4" s="39"/>
+      <c r="Q4" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="R4" s="39"/>
+      <c r="S4" s="39"/>
+      <c r="T4" s="39"/>
+      <c r="U4" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="V4" s="69"/>
+    </row>
+    <row r="5" spans="2:23" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B5" s="29"/>
+      <c r="C5" s="70" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="70" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="70" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" s="70" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" s="70" t="s">
+        <v>45</v>
+      </c>
+      <c r="H5" s="70" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" s="70" t="s">
+        <v>48</v>
+      </c>
+      <c r="J5" s="70" t="s">
+        <v>49</v>
+      </c>
+      <c r="K5" s="70" t="s">
+        <v>52</v>
+      </c>
+      <c r="L5" s="70" t="s">
+        <v>65</v>
+      </c>
+      <c r="M5" s="67" t="s">
+        <v>62</v>
+      </c>
+      <c r="N5" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="O5" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="P5" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q5" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="R5" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="S5" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="T5" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="U5" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="V5" s="71" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:23" x14ac:dyDescent="0.4">
+      <c r="B6" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="35">
+        <v>4.99</v>
+      </c>
+      <c r="G6" s="35">
+        <v>1</v>
+      </c>
+      <c r="H6" s="35">
+        <f>1+F6/G6</f>
+        <v>5.99</v>
+      </c>
+      <c r="I6" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="J6" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="K6" s="35">
+        <v>0</v>
+      </c>
+      <c r="L6" s="80">
+        <v>10000</v>
+      </c>
+      <c r="M6" s="35"/>
+      <c r="N6" s="35">
+        <v>0.6</v>
+      </c>
+      <c r="O6" s="35">
+        <v>0.52</v>
+      </c>
+      <c r="P6" s="35">
+        <v>0.16</v>
+      </c>
+      <c r="Q6" s="35">
+        <v>2.64</v>
+      </c>
+      <c r="R6" s="35">
+        <v>0.9</v>
+      </c>
+      <c r="S6" s="35">
+        <f>R6/L6*1000</f>
+        <v>9.0000000000000011E-2</v>
+      </c>
+      <c r="T6" s="72">
+        <f>R6*R6/L6*1000</f>
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="U6" s="36">
+        <f>Q6/O6</f>
+        <v>5.0769230769230766</v>
+      </c>
+      <c r="V6" s="73">
+        <f>R6/P6</f>
+        <v>5.625</v>
+      </c>
+    </row>
+    <row r="7" spans="2:23" x14ac:dyDescent="0.4">
+      <c r="B7" s="9"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4">
+        <v>0</v>
+      </c>
+      <c r="J7" s="4">
+        <v>0</v>
+      </c>
+      <c r="K7" s="4">
+        <v>0</v>
+      </c>
+      <c r="L7" s="81">
+        <v>10000</v>
+      </c>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4">
+        <v>12</v>
+      </c>
+      <c r="R7" s="4">
+        <v>12</v>
+      </c>
+      <c r="S7" s="4"/>
+      <c r="T7" s="4"/>
+      <c r="U7" s="4"/>
+      <c r="V7" s="74"/>
+      <c r="W7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="2:23" x14ac:dyDescent="0.4">
+      <c r="B8" s="9"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4">
+        <v>49.9</v>
+      </c>
+      <c r="L8" s="82">
+        <v>49.9</v>
+      </c>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="O8" s="4">
+        <v>0.52</v>
+      </c>
+      <c r="P8" s="4">
+        <v>0.158</v>
+      </c>
+      <c r="Q8" s="4">
+        <v>1.24</v>
+      </c>
+      <c r="R8" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="S8" s="65">
+        <f>R8/L8*1000</f>
+        <v>8.0160320641282574</v>
+      </c>
+      <c r="T8" s="65">
+        <f>R8*R8/L8*1000</f>
+        <v>3.2064128256513036</v>
+      </c>
+      <c r="U8" s="66">
+        <f t="shared" ref="U8:V11" si="0">Q8/O8</f>
+        <v>2.3846153846153846</v>
+      </c>
+      <c r="V8" s="75">
+        <f t="shared" si="0"/>
+        <v>2.5316455696202533</v>
+      </c>
+    </row>
+    <row r="9" spans="2:23" x14ac:dyDescent="0.4">
+      <c r="B9" s="9"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4">
+        <v>0</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="O9" s="4">
+        <v>0.52</v>
+      </c>
+      <c r="P9" s="4">
+        <v>0.158</v>
+      </c>
+      <c r="Q9" s="4">
+        <v>2.6</v>
+      </c>
+      <c r="R9" s="4">
+        <v>0.88900000000000001</v>
+      </c>
+      <c r="S9" s="4"/>
+      <c r="T9" s="4"/>
+      <c r="U9" s="66">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="V9" s="75">
+        <f t="shared" si="0"/>
+        <v>5.6265822784810124</v>
+      </c>
+    </row>
+    <row r="10" spans="2:23" x14ac:dyDescent="0.4">
+      <c r="B10" s="9"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="O10" s="4">
+        <v>0.52</v>
+      </c>
+      <c r="P10" s="4">
+        <v>0.158</v>
+      </c>
+      <c r="Q10" s="4">
+        <v>2.64</v>
+      </c>
+      <c r="R10" s="4">
+        <v>0.90700000000000003</v>
+      </c>
+      <c r="S10" s="4"/>
+      <c r="T10" s="4"/>
+      <c r="U10" s="66">
+        <f t="shared" si="0"/>
+        <v>5.0769230769230766</v>
+      </c>
+      <c r="V10" s="75">
+        <f t="shared" si="0"/>
+        <v>5.7405063291139244</v>
+      </c>
+    </row>
+    <row r="11" spans="2:23" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B11" s="29"/>
+      <c r="C11" s="70"/>
+      <c r="D11" s="70"/>
+      <c r="E11" s="70"/>
+      <c r="F11" s="76">
+        <v>4.99</v>
+      </c>
+      <c r="G11" s="76">
+        <v>0.80600000000000005</v>
+      </c>
+      <c r="H11" s="77">
+        <f>1+F11/G11</f>
+        <v>7.1910669975186101</v>
+      </c>
+      <c r="I11" s="70"/>
+      <c r="J11" s="70"/>
+      <c r="K11" s="70"/>
+      <c r="L11" s="70"/>
+      <c r="M11" s="70"/>
+      <c r="N11" s="70">
+        <v>0.6</v>
+      </c>
+      <c r="O11" s="70">
+        <v>0.52</v>
+      </c>
+      <c r="P11" s="70">
+        <v>0.158</v>
+      </c>
+      <c r="Q11" s="70">
+        <v>2.76</v>
+      </c>
+      <c r="R11" s="70">
+        <v>0.94</v>
+      </c>
+      <c r="S11" s="70"/>
+      <c r="T11" s="70"/>
+      <c r="U11" s="78">
+        <f t="shared" si="0"/>
+        <v>5.3076923076923075</v>
+      </c>
+      <c r="V11" s="79">
+        <f t="shared" si="0"/>
+        <v>5.9493670886075947</v>
+      </c>
+    </row>
+    <row r="12" spans="2:23" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B12" s="83" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" s="84" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="84" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="84" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="84">
+        <v>510</v>
+      </c>
+      <c r="G12" s="84" t="s">
+        <v>67</v>
+      </c>
+      <c r="H12" s="84" t="e">
+        <f>1+F12/G12</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I12" s="84" t="s">
+        <v>67</v>
+      </c>
+      <c r="J12" s="84" t="s">
+        <v>67</v>
+      </c>
+      <c r="K12" s="4">
+        <v>49.9</v>
+      </c>
+      <c r="L12" s="84" t="s">
+        <v>67</v>
+      </c>
+      <c r="M12" s="82">
+        <v>49.9</v>
+      </c>
+      <c r="N12" s="84">
+        <v>0.6</v>
+      </c>
+      <c r="O12" s="84">
+        <v>0.57599999999999996</v>
+      </c>
+      <c r="P12" s="84">
+        <v>0.19600000000000001</v>
+      </c>
+      <c r="Q12" s="84">
+        <v>0.504</v>
+      </c>
+      <c r="R12" s="84">
+        <v>0.17</v>
+      </c>
+      <c r="S12" s="85">
+        <f>R12/M12*1000</f>
+        <v>3.4068136272545093</v>
+      </c>
+      <c r="T12" s="85">
+        <f>R12*R12/M12*1000</f>
+        <v>0.57915831663326667</v>
+      </c>
+      <c r="U12" s="86">
+        <f>Q12/O12</f>
+        <v>0.87500000000000011</v>
+      </c>
+      <c r="V12" s="87">
+        <f>R12/P12</f>
+        <v>0.86734693877551028</v>
+      </c>
+    </row>
+    <row r="13" spans="2:23" x14ac:dyDescent="0.4">
+      <c r="B13" s="83" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" s="84" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="84" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="84" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" s="84">
+        <v>510</v>
+      </c>
+      <c r="G13" s="4">
+        <v>49.9</v>
+      </c>
+      <c r="H13" s="86">
+        <f>1+F13/G13</f>
+        <v>11.220440881763528</v>
+      </c>
+      <c r="I13" s="84" t="s">
+        <v>68</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K13" s="4">
+        <v>49.9</v>
+      </c>
+      <c r="L13" s="84" t="s">
+        <v>67</v>
+      </c>
+      <c r="M13" s="84" t="s">
+        <v>67</v>
+      </c>
+      <c r="N13" s="84">
+        <v>0.6</v>
+      </c>
+      <c r="O13" s="84">
+        <v>0.57599999999999996</v>
+      </c>
+      <c r="P13" s="84">
+        <v>0.19600000000000001</v>
+      </c>
+      <c r="Q13" s="84">
+        <v>2.68</v>
+      </c>
+      <c r="R13" s="84">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="S13" s="85" t="e">
+        <f>R13/M13*1000</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="T13" s="85" t="e">
+        <f>R13*R13/M13*1000</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="U13" s="86">
+        <f>Q13/O13</f>
+        <v>4.6527777777777786</v>
+      </c>
+      <c r="V13" s="87">
+        <f>R13/P13</f>
+        <v>4.7295918367346941</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="Q4:T4"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30B35F9E-DE43-4A16-A003-225CBE2BE0BE}">
+  <dimension ref="B3:W14"/>
+  <sheetViews>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="2.3984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:23" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="4" spans="2:23" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B4" s="26"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="68" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="68"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
+      <c r="H4" s="67"/>
+      <c r="I4" s="67"/>
+      <c r="J4" s="67"/>
+      <c r="K4" s="67"/>
+      <c r="M4" s="67"/>
+      <c r="N4" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="O4" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="P4" s="39"/>
+      <c r="Q4" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="R4" s="39"/>
+      <c r="S4" s="39"/>
+      <c r="T4" s="39"/>
+      <c r="U4" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="V4" s="69"/>
+    </row>
+    <row r="5" spans="2:23" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B5" s="29"/>
+      <c r="C5" s="70" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="70" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="70" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" s="70" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" s="70" t="s">
+        <v>45</v>
+      </c>
+      <c r="H5" s="70" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" s="70" t="s">
+        <v>48</v>
+      </c>
+      <c r="J5" s="70" t="s">
+        <v>49</v>
+      </c>
+      <c r="K5" s="70" t="s">
+        <v>52</v>
+      </c>
+      <c r="L5" s="70" t="s">
+        <v>65</v>
+      </c>
+      <c r="M5" s="67" t="s">
+        <v>62</v>
+      </c>
+      <c r="N5" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="O5" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="P5" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q5" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="R5" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="S5" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="T5" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="U5" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="V5" s="71" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:23" x14ac:dyDescent="0.4">
+      <c r="B6" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="35">
+        <v>4.99</v>
+      </c>
+      <c r="G6" s="35">
+        <v>1</v>
+      </c>
+      <c r="H6" s="35">
+        <f>1+F6/G6</f>
+        <v>5.99</v>
+      </c>
+      <c r="I6" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="J6" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="K6" s="35">
+        <v>0</v>
+      </c>
+      <c r="L6" s="80">
+        <v>10000</v>
+      </c>
+      <c r="M6" s="35"/>
+      <c r="N6" s="35">
+        <v>0.6</v>
+      </c>
+      <c r="O6" s="35">
+        <v>0.52</v>
+      </c>
+      <c r="P6" s="35">
+        <v>0.16</v>
+      </c>
+      <c r="Q6" s="35">
+        <v>2.64</v>
+      </c>
+      <c r="R6" s="35">
+        <v>0.9</v>
+      </c>
+      <c r="S6" s="35">
+        <f>R6/L6*1000</f>
+        <v>9.0000000000000011E-2</v>
+      </c>
+      <c r="T6" s="72">
+        <f>R6*R6/L6*1000</f>
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="U6" s="36">
+        <f>Q6/O6</f>
+        <v>5.0769230769230766</v>
+      </c>
+      <c r="V6" s="73">
+        <f>R6/P6</f>
+        <v>5.625</v>
+      </c>
+    </row>
+    <row r="7" spans="2:23" x14ac:dyDescent="0.4">
+      <c r="B7" s="9"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4">
+        <v>0</v>
+      </c>
+      <c r="J7" s="4">
+        <v>0</v>
+      </c>
+      <c r="K7" s="4">
+        <v>0</v>
+      </c>
+      <c r="L7" s="81">
+        <v>10000</v>
+      </c>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4">
+        <v>12</v>
+      </c>
+      <c r="R7" s="4">
+        <v>12</v>
+      </c>
+      <c r="S7" s="4"/>
+      <c r="T7" s="4"/>
+      <c r="U7" s="4"/>
+      <c r="V7" s="74"/>
+      <c r="W7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="2:23" x14ac:dyDescent="0.4">
+      <c r="B8" s="9"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4">
+        <v>49.9</v>
+      </c>
+      <c r="L8" s="82">
+        <v>49.9</v>
+      </c>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="O8" s="4">
+        <v>0.52</v>
+      </c>
+      <c r="P8" s="4">
+        <v>0.158</v>
+      </c>
+      <c r="Q8" s="4">
+        <v>1.24</v>
+      </c>
+      <c r="R8" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="S8" s="65">
+        <f>R8/L8*1000</f>
+        <v>8.0160320641282574</v>
+      </c>
+      <c r="T8" s="65">
+        <f>R8*R8/L8*1000</f>
+        <v>3.2064128256513036</v>
+      </c>
+      <c r="U8" s="66">
+        <f t="shared" ref="U8:V11" si="0">Q8/O8</f>
+        <v>2.3846153846153846</v>
+      </c>
+      <c r="V8" s="75">
+        <f t="shared" si="0"/>
+        <v>2.5316455696202533</v>
+      </c>
+    </row>
+    <row r="9" spans="2:23" x14ac:dyDescent="0.4">
+      <c r="B9" s="9"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4">
+        <v>0</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="O9" s="4">
+        <v>0.52</v>
+      </c>
+      <c r="P9" s="4">
+        <v>0.158</v>
+      </c>
+      <c r="Q9" s="4">
+        <v>2.6</v>
+      </c>
+      <c r="R9" s="4">
+        <v>0.88900000000000001</v>
+      </c>
+      <c r="S9" s="4"/>
+      <c r="T9" s="4"/>
+      <c r="U9" s="66">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="V9" s="75">
+        <f t="shared" si="0"/>
+        <v>5.6265822784810124</v>
+      </c>
+    </row>
+    <row r="10" spans="2:23" x14ac:dyDescent="0.4">
+      <c r="B10" s="9"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="O10" s="4">
+        <v>0.52</v>
+      </c>
+      <c r="P10" s="4">
+        <v>0.158</v>
+      </c>
+      <c r="Q10" s="4">
+        <v>2.64</v>
+      </c>
+      <c r="R10" s="4">
+        <v>0.90700000000000003</v>
+      </c>
+      <c r="S10" s="4"/>
+      <c r="T10" s="4"/>
+      <c r="U10" s="66">
+        <f t="shared" si="0"/>
+        <v>5.0769230769230766</v>
+      </c>
+      <c r="V10" s="75">
+        <f t="shared" si="0"/>
+        <v>5.7405063291139244</v>
+      </c>
+    </row>
+    <row r="11" spans="2:23" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B11" s="29"/>
+      <c r="C11" s="70"/>
+      <c r="D11" s="70"/>
+      <c r="E11" s="70"/>
+      <c r="F11" s="76">
+        <v>4.99</v>
+      </c>
+      <c r="G11" s="76">
+        <v>0.80600000000000005</v>
+      </c>
+      <c r="H11" s="77">
+        <f>1+F11/G11</f>
+        <v>7.1910669975186101</v>
+      </c>
+      <c r="I11" s="70"/>
+      <c r="J11" s="70"/>
+      <c r="K11" s="70"/>
+      <c r="L11" s="70"/>
+      <c r="M11" s="70"/>
+      <c r="N11" s="70">
+        <v>0.6</v>
+      </c>
+      <c r="O11" s="70">
+        <v>0.52</v>
+      </c>
+      <c r="P11" s="70">
+        <v>0.158</v>
+      </c>
+      <c r="Q11" s="70">
+        <v>2.76</v>
+      </c>
+      <c r="R11" s="70">
+        <v>0.94</v>
+      </c>
+      <c r="S11" s="70"/>
+      <c r="T11" s="70"/>
+      <c r="U11" s="78">
+        <f t="shared" si="0"/>
+        <v>5.3076923076923075</v>
+      </c>
+      <c r="V11" s="79">
+        <f t="shared" si="0"/>
+        <v>5.9493670886075947</v>
+      </c>
+    </row>
+    <row r="12" spans="2:23" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B12" s="83" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" s="84" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="84" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="84" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="84">
+        <v>510</v>
+      </c>
+      <c r="G12" s="84" t="s">
+        <v>67</v>
+      </c>
+      <c r="H12" s="84" t="e">
+        <f>1+F12/G12</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I12" s="84" t="s">
+        <v>67</v>
+      </c>
+      <c r="J12" s="84" t="s">
+        <v>67</v>
+      </c>
+      <c r="K12" s="4">
+        <v>49.9</v>
+      </c>
+      <c r="L12" s="84" t="s">
+        <v>67</v>
+      </c>
+      <c r="M12" s="82">
+        <v>49.9</v>
+      </c>
+      <c r="N12" s="84">
+        <v>0.6</v>
+      </c>
+      <c r="O12" s="84">
+        <v>0.57599999999999996</v>
+      </c>
+      <c r="P12" s="84">
+        <v>0.19600000000000001</v>
+      </c>
+      <c r="Q12" s="84">
+        <v>0.504</v>
+      </c>
+      <c r="R12" s="84">
+        <v>0.17</v>
+      </c>
+      <c r="S12" s="85">
+        <f>R12/M12*1000</f>
+        <v>3.4068136272545093</v>
+      </c>
+      <c r="T12" s="85">
+        <f>R12*R12/M12*1000</f>
+        <v>0.57915831663326667</v>
+      </c>
+      <c r="U12" s="86">
+        <f>Q12/O12</f>
+        <v>0.87500000000000011</v>
+      </c>
+      <c r="V12" s="87">
+        <f>R12/P12</f>
+        <v>0.86734693877551028</v>
+      </c>
+    </row>
+    <row r="13" spans="2:23" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B13" s="83" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" s="84" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="84" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="84" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" s="84">
+        <v>510</v>
+      </c>
+      <c r="G13" s="4">
+        <v>49.9</v>
+      </c>
+      <c r="H13" s="86">
+        <f>1+F13/G13</f>
+        <v>11.220440881763528</v>
+      </c>
+      <c r="I13" s="84" t="s">
+        <v>68</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K13" s="4">
+        <v>49.9</v>
+      </c>
+      <c r="L13" s="84" t="s">
+        <v>67</v>
+      </c>
+      <c r="M13" s="84" t="s">
+        <v>67</v>
+      </c>
+      <c r="N13" s="84">
+        <v>0.6</v>
+      </c>
+      <c r="O13" s="84">
+        <v>0.496</v>
+      </c>
+      <c r="P13" s="84">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="Q13" s="84">
+        <v>2.68</v>
+      </c>
+      <c r="R13" s="84">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="S13" s="85" t="e">
+        <f>R13/M13*1000</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="T13" s="85" t="e">
+        <f>R13*R13/M13*1000</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="U13" s="86">
+        <f>Q13/O13</f>
+        <v>5.403225806451613</v>
+      </c>
+      <c r="V13" s="87">
+        <f>R13/P13</f>
+        <v>5.6871165644171784</v>
+      </c>
+    </row>
+    <row r="14" spans="2:23" x14ac:dyDescent="0.4">
+      <c r="N14" s="84">
+        <v>0.6</v>
+      </c>
+      <c r="O14" s="84">
+        <v>0.57599999999999996</v>
+      </c>
+      <c r="P14" s="84">
+        <v>0.19600000000000001</v>
+      </c>
+      <c r="Q14" s="84">
+        <v>2.68</v>
+      </c>
+      <c r="R14" s="84">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="S14" s="85" t="e">
+        <f>R14/M14*1000</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T14" s="85" t="e">
+        <f>R14*R14/M14*1000</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U14" s="86">
+        <f>Q14/O14</f>
+        <v>4.6527777777777786</v>
+      </c>
+      <c r="V14" s="87">
+        <f>R14/P14</f>
+        <v>4.7295918367346941</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="Q4:T4"/>
+    <mergeCell ref="U4:V4"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:S25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -998,7 +2566,7 @@
       <c r="G2">
         <v>4</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1021,512 +2589,512 @@
       <c r="G3">
         <v>100000</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="C4" s="3">
+    <row r="4" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="C4" s="2">
         <f>1/(2*3.14*C2*C3/1000000)</f>
         <v>11.373976342129209</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <f>1/(2*3.14*D2*D3/1000000)</f>
         <v>113.7397634212921</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <f>1/(2*3.14*E2*E3/1000000)</f>
         <v>568.69881710646041</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <f>1/(2*3.14*F2*F3/1000000)</f>
         <v>3.9808917197452232</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="2">
         <f>1/(2*3.14*G2*G3/1000000)</f>
         <v>0.39808917197452232</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:17" s="3" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
-    <row r="7" spans="1:17" s="3" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B7" s="4" t="s">
+    <row r="6" spans="1:17" s="2" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="7" spans="1:17" s="2" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="K7" s="20" t="s">
+      <c r="C7" s="3"/>
+      <c r="K7" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="L7" s="21" t="s">
+      <c r="L7" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="M7" s="21"/>
-      <c r="N7" s="21" t="s">
+      <c r="M7" s="42"/>
+      <c r="N7" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="O7" s="21"/>
-      <c r="P7" s="21" t="s">
+      <c r="O7" s="42"/>
+      <c r="P7" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="Q7" s="22"/>
-    </row>
-    <row r="8" spans="1:17" s="3" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B8" s="20"/>
-      <c r="C8" s="29" t="s">
+      <c r="Q7" s="43"/>
+    </row>
+    <row r="8" spans="1:17" s="2" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B8" s="17"/>
+      <c r="C8" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="29" t="s">
+      <c r="D8" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="29" t="s">
+      <c r="E8" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="29" t="s">
+      <c r="F8" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="29" t="s">
+      <c r="G8" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="H8" s="29" t="s">
+      <c r="H8" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="I8" s="29" t="s">
+      <c r="I8" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="J8" s="29" t="s">
+      <c r="J8" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="K8" s="29" t="s">
+      <c r="K8" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="L8" s="29" t="s">
+      <c r="L8" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="M8" s="29" t="s">
+      <c r="M8" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="N8" s="29" t="s">
+      <c r="N8" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="O8" s="29" t="s">
+      <c r="O8" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="P8" s="29" t="s">
+      <c r="P8" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="Q8" s="30" t="s">
+      <c r="Q8" s="25" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="24" t="s">
+      <c r="D9" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="E9" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="24">
+      <c r="F9" s="19">
         <v>680</v>
       </c>
-      <c r="G9" s="24">
+      <c r="G9" s="19">
         <v>680</v>
       </c>
-      <c r="H9" s="24">
+      <c r="H9" s="19">
         <f>1+F9/G9</f>
         <v>2</v>
       </c>
-      <c r="I9" s="24" t="s">
+      <c r="I9" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="J9" s="24">
+      <c r="J9" s="19">
         <v>51</v>
       </c>
-      <c r="K9" s="25">
+      <c r="K9" s="20">
         <v>1</v>
       </c>
-      <c r="L9" s="26"/>
-      <c r="M9" s="26"/>
-      <c r="N9" s="26">
+      <c r="L9" s="21"/>
+      <c r="M9" s="21"/>
+      <c r="N9" s="21">
         <v>2</v>
       </c>
-      <c r="O9" s="27">
+      <c r="O9" s="22">
         <v>0.65500000000000003</v>
       </c>
-      <c r="P9" s="26" t="e">
+      <c r="P9" s="21" t="e">
         <f>N9/L9</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q9" s="28" t="e">
+      <c r="Q9" s="23" t="e">
         <f>O9/M9</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="B10" s="12"/>
-      <c r="C10" s="8" t="s">
+      <c r="B10" s="9"/>
+      <c r="C10" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F10" s="5">
         <v>680</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="5">
         <v>680</v>
       </c>
-      <c r="H10" s="8">
+      <c r="H10" s="5">
         <f>1+F10/G10</f>
         <v>2</v>
       </c>
-      <c r="I10" s="8" t="s">
+      <c r="I10" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="J10" s="8">
+      <c r="J10" s="5">
         <v>51</v>
       </c>
-      <c r="K10" s="7">
+      <c r="K10" s="4">
         <v>1</v>
       </c>
-      <c r="L10" s="9">
+      <c r="L10" s="6">
         <v>1</v>
       </c>
-      <c r="M10" s="10">
+      <c r="M10" s="7">
         <v>0.3</v>
       </c>
-      <c r="N10" s="9">
+      <c r="N10" s="6">
         <v>2.16</v>
       </c>
-      <c r="O10" s="10">
+      <c r="O10" s="7">
         <v>0.7</v>
       </c>
-      <c r="P10" s="9">
+      <c r="P10" s="6">
         <f t="shared" ref="P10" si="0">N10/L10</f>
         <v>2.16</v>
       </c>
-      <c r="Q10" s="13">
+      <c r="Q10" s="10">
         <f t="shared" ref="Q10" si="1">O10/M10</f>
         <v>2.3333333333333335</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="B11" s="12"/>
-      <c r="C11" s="8" t="s">
+      <c r="B11" s="9"/>
+      <c r="C11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F11" s="5">
         <v>680</v>
       </c>
-      <c r="G11" s="8">
+      <c r="G11" s="5">
         <v>680</v>
       </c>
-      <c r="H11" s="8">
+      <c r="H11" s="5">
         <f t="shared" ref="H11:H16" si="2">1+F11/G11</f>
         <v>2</v>
       </c>
-      <c r="I11" s="8" t="s">
+      <c r="I11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="J11" s="8">
+      <c r="J11" s="5">
         <v>51</v>
       </c>
-      <c r="K11" s="7">
+      <c r="K11" s="4">
         <v>1</v>
       </c>
-      <c r="L11" s="9">
+      <c r="L11" s="6">
         <v>1</v>
       </c>
-      <c r="M11" s="10">
+      <c r="M11" s="7">
         <v>0.3</v>
       </c>
-      <c r="N11" s="9">
+      <c r="N11" s="6">
         <v>2.16</v>
       </c>
-      <c r="O11" s="10">
+      <c r="O11" s="7">
         <v>0.69499999999999995</v>
       </c>
-      <c r="P11" s="9">
+      <c r="P11" s="6">
         <f t="shared" ref="P11:P12" si="3">N11/L11</f>
         <v>2.16</v>
       </c>
-      <c r="Q11" s="13">
+      <c r="Q11" s="10">
         <f t="shared" ref="Q11:Q12" si="4">O11/M11</f>
         <v>2.3166666666666664</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="B12" s="12"/>
-      <c r="C12" s="8" t="s">
+      <c r="B12" s="9"/>
+      <c r="C12" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F12" s="5">
         <v>680</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G12" s="5">
         <v>680</v>
       </c>
-      <c r="H12" s="8">
+      <c r="H12" s="5">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="I12" s="8" t="s">
+      <c r="I12" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="J12" s="8">
+      <c r="J12" s="5">
         <v>51</v>
       </c>
-      <c r="K12" s="7">
+      <c r="K12" s="4">
         <v>3</v>
       </c>
-      <c r="L12" s="9">
+      <c r="L12" s="6">
         <v>2.68</v>
       </c>
-      <c r="M12" s="10">
+      <c r="M12" s="7">
         <v>0.9</v>
       </c>
-      <c r="N12" s="9">
+      <c r="N12" s="6">
         <v>5.88</v>
       </c>
-      <c r="O12" s="10">
+      <c r="O12" s="7">
         <v>2.02</v>
       </c>
-      <c r="P12" s="9">
+      <c r="P12" s="6">
         <f t="shared" si="3"/>
         <v>2.1940298507462686</v>
       </c>
-      <c r="Q12" s="13">
+      <c r="Q12" s="10">
         <f t="shared" si="4"/>
         <v>2.2444444444444445</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="B13" s="12"/>
-      <c r="C13" s="8">
+      <c r="B13" s="9"/>
+      <c r="C13" s="5">
         <v>49.9</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F13" s="5">
         <v>680</v>
       </c>
-      <c r="G13" s="8">
+      <c r="G13" s="5">
         <v>680</v>
       </c>
-      <c r="H13" s="8">
+      <c r="H13" s="5">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="I13" s="8" t="s">
+      <c r="I13" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="J13" s="8">
+      <c r="J13" s="5">
         <v>51</v>
       </c>
-      <c r="K13" s="7">
+      <c r="K13" s="4">
         <v>3</v>
       </c>
-      <c r="L13" s="9">
+      <c r="L13" s="6">
         <v>1.2</v>
       </c>
-      <c r="M13" s="10">
+      <c r="M13" s="7">
         <v>0.38</v>
       </c>
-      <c r="N13" s="9">
+      <c r="N13" s="6">
         <v>2.56</v>
       </c>
-      <c r="O13" s="10">
+      <c r="O13" s="7">
         <v>0.88</v>
       </c>
-      <c r="P13" s="9">
-        <f>N13/L13</f>
+      <c r="P13" s="6">
+        <f t="shared" ref="P13:Q16" si="5">N13/L13</f>
         <v>2.1333333333333333</v>
       </c>
-      <c r="Q13" s="13">
-        <f>O13/M13</f>
+      <c r="Q13" s="10">
+        <f t="shared" si="5"/>
         <v>2.3157894736842106</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="B14" s="12"/>
-      <c r="C14" s="8" t="s">
+      <c r="B14" s="9"/>
+      <c r="C14" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="E14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="8">
+      <c r="F14" s="5">
         <v>680</v>
       </c>
-      <c r="G14" s="8">
+      <c r="G14" s="5">
         <v>680</v>
       </c>
-      <c r="H14" s="8">
+      <c r="H14" s="5">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="I14" s="8" t="s">
+      <c r="I14" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="J14" s="8">
+      <c r="J14" s="5">
         <v>51</v>
       </c>
-      <c r="K14" s="7">
+      <c r="K14" s="4">
         <v>1</v>
       </c>
-      <c r="L14" s="9">
+      <c r="L14" s="6">
         <v>1.04</v>
       </c>
-      <c r="M14" s="10">
+      <c r="M14" s="7">
         <v>0.3</v>
       </c>
-      <c r="N14" s="9">
+      <c r="N14" s="6">
         <v>2.2000000000000002</v>
       </c>
-      <c r="O14" s="10">
+      <c r="O14" s="7">
         <v>0.71</v>
       </c>
-      <c r="P14" s="9">
-        <f>N14/L14</f>
+      <c r="P14" s="6">
+        <f t="shared" si="5"/>
         <v>2.1153846153846154</v>
       </c>
-      <c r="Q14" s="13">
-        <f>O14/M14</f>
+      <c r="Q14" s="10">
+        <f t="shared" si="5"/>
         <v>2.3666666666666667</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="B15" s="12"/>
-      <c r="C15" s="8" t="s">
+      <c r="B15" s="9"/>
+      <c r="C15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F15" s="8">
+      <c r="F15" s="5">
         <v>680</v>
       </c>
-      <c r="G15" s="8">
+      <c r="G15" s="5">
         <v>680</v>
       </c>
-      <c r="H15" s="8">
+      <c r="H15" s="5">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="I15" s="8" t="s">
+      <c r="I15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="J15" s="8">
+      <c r="J15" s="5">
         <v>51</v>
       </c>
-      <c r="K15" s="7">
+      <c r="K15" s="4">
         <v>3</v>
       </c>
-      <c r="L15" s="9">
+      <c r="L15" s="6">
         <v>2.72</v>
       </c>
-      <c r="M15" s="10">
+      <c r="M15" s="7">
         <v>0.9</v>
       </c>
-      <c r="N15" s="9">
+      <c r="N15" s="6">
         <v>5.92</v>
       </c>
-      <c r="O15" s="10">
+      <c r="O15" s="7">
         <v>2.04</v>
       </c>
-      <c r="P15" s="9">
-        <f>N15/L15</f>
+      <c r="P15" s="6">
+        <f t="shared" si="5"/>
         <v>2.1764705882352939</v>
       </c>
-      <c r="Q15" s="13">
-        <f>O15/M15</f>
+      <c r="Q15" s="10">
+        <f t="shared" si="5"/>
         <v>2.2666666666666666</v>
       </c>
     </row>
     <row r="16" spans="1:17" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="15" t="s">
+      <c r="D16" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E16" s="15" t="s">
+      <c r="E16" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="15">
+      <c r="F16" s="12">
         <v>680</v>
       </c>
-      <c r="G16" s="15">
+      <c r="G16" s="12">
         <v>680</v>
       </c>
-      <c r="H16" s="15">
+      <c r="H16" s="12">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="I16" s="15" t="s">
+      <c r="I16" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="J16" s="15">
+      <c r="J16" s="12">
         <v>51</v>
       </c>
-      <c r="K16" s="16">
+      <c r="K16" s="13">
         <v>3</v>
       </c>
-      <c r="L16" s="17">
+      <c r="L16" s="14">
         <v>2.7</v>
       </c>
-      <c r="M16" s="18">
+      <c r="M16" s="15">
         <v>0.91</v>
       </c>
-      <c r="N16" s="17">
+      <c r="N16" s="14">
         <v>6</v>
       </c>
-      <c r="O16" s="18">
+      <c r="O16" s="15">
         <v>2.0699999999999998</v>
       </c>
-      <c r="P16" s="17">
-        <f>N16/L16</f>
+      <c r="P16" s="14">
+        <f t="shared" si="5"/>
         <v>2.2222222222222219</v>
       </c>
-      <c r="Q16" s="19">
-        <f>O16/M16</f>
+      <c r="Q16" s="16">
+        <f t="shared" si="5"/>
         <v>2.2747252747252746</v>
       </c>
     </row>
@@ -1541,7 +3109,7 @@
       <c r="J17" s="1"/>
     </row>
     <row r="18" spans="2:19" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C18" s="1"/>
@@ -1554,295 +3122,295 @@
       <c r="J18" s="1"/>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.4">
-      <c r="B19" s="31"/>
-      <c r="C19" s="32"/>
-      <c r="D19" s="32"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="32"/>
-      <c r="H19" s="11" t="s">
+      <c r="B19" s="26"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="I19" s="33" t="s">
+      <c r="I19" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="J19" s="33"/>
-      <c r="K19" s="33" t="s">
+      <c r="J19" s="39"/>
+      <c r="K19" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="L19" s="33"/>
-      <c r="M19" s="33" t="s">
+      <c r="L19" s="39"/>
+      <c r="M19" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="N19" s="33"/>
-      <c r="O19" s="33" t="s">
+      <c r="N19" s="39"/>
+      <c r="O19" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="P19" s="33"/>
-      <c r="Q19" s="33" t="s">
+      <c r="P19" s="39"/>
+      <c r="Q19" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="R19" s="33"/>
-      <c r="S19" s="34" t="s">
+      <c r="R19" s="39"/>
+      <c r="S19" s="40" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="20" spans="2:19" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B20" s="35"/>
-      <c r="C20" s="36" t="s">
+      <c r="B20" s="29"/>
+      <c r="C20" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="36" t="s">
+      <c r="D20" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="E20" s="37" t="s">
+      <c r="E20" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="F20" s="37" t="s">
+      <c r="F20" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="G20" s="37" t="s">
+      <c r="G20" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="H20" s="36" t="s">
+      <c r="H20" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="I20" s="36" t="s">
+      <c r="I20" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="J20" s="36" t="s">
+      <c r="J20" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="K20" s="36" t="s">
+      <c r="K20" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="L20" s="36" t="s">
+      <c r="L20" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="M20" s="36" t="s">
+      <c r="M20" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="N20" s="36" t="s">
+      <c r="N20" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="O20" s="36" t="s">
+      <c r="O20" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="P20" s="36" t="s">
+      <c r="P20" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="Q20" s="36" t="s">
+      <c r="Q20" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="R20" s="36" t="s">
+      <c r="R20" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="S20" s="38"/>
+      <c r="S20" s="41"/>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.4">
-      <c r="B21" s="40" t="s">
+      <c r="B21" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="41" t="s">
+      <c r="C21" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="D21" s="41">
+      <c r="D21" s="34">
         <v>0</v>
       </c>
-      <c r="E21" s="41" t="s">
+      <c r="E21" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="F21" s="41">
+      <c r="F21" s="34">
         <v>51</v>
       </c>
-      <c r="G21" s="41" t="s">
+      <c r="G21" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="H21" s="42">
+      <c r="H21" s="35">
         <v>3</v>
       </c>
-      <c r="I21" s="42">
+      <c r="I21" s="35">
         <v>2.8</v>
       </c>
-      <c r="J21" s="42">
+      <c r="J21" s="35">
         <v>0.95</v>
       </c>
-      <c r="K21" s="42">
+      <c r="K21" s="35">
         <v>6.12</v>
       </c>
-      <c r="L21" s="42">
+      <c r="L21" s="35">
         <v>2.1</v>
       </c>
-      <c r="M21" s="43">
+      <c r="M21" s="36">
         <f>K21/I21</f>
         <v>2.1857142857142859</v>
       </c>
-      <c r="N21" s="43">
+      <c r="N21" s="36">
         <f>L21/J21</f>
         <v>2.2105263157894739</v>
       </c>
-      <c r="O21" s="42">
+      <c r="O21" s="35">
         <v>1.52</v>
       </c>
-      <c r="P21" s="42">
+      <c r="P21" s="35">
         <v>0.495</v>
       </c>
-      <c r="Q21" s="42">
+      <c r="Q21" s="35">
         <v>3.04</v>
       </c>
-      <c r="R21" s="42">
+      <c r="R21" s="35">
         <v>1.03</v>
       </c>
-      <c r="S21" s="44">
+      <c r="S21" s="37">
         <f>O21/Q21</f>
         <v>0.5</v>
       </c>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.4">
-      <c r="B22" s="12"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="7" t="s">
+      <c r="B22" s="9"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G22" s="8"/>
-      <c r="H22" s="7">
+      <c r="G22" s="5"/>
+      <c r="H22" s="4">
         <v>3</v>
       </c>
-      <c r="I22" s="7">
+      <c r="I22" s="4">
         <v>2.8</v>
       </c>
-      <c r="J22" s="7">
+      <c r="J22" s="4">
         <v>0.95</v>
       </c>
-      <c r="K22" s="7">
+      <c r="K22" s="4">
         <v>6</v>
       </c>
-      <c r="L22" s="7">
+      <c r="L22" s="4">
         <v>2.04</v>
       </c>
-      <c r="M22" s="9">
+      <c r="M22" s="6">
         <f>K22/I22</f>
         <v>2.1428571428571428</v>
       </c>
-      <c r="N22" s="9">
+      <c r="N22" s="6">
         <f>L22/J22</f>
         <v>2.1473684210526316</v>
       </c>
-      <c r="O22" s="7">
+      <c r="O22" s="4">
         <v>2.44</v>
       </c>
-      <c r="P22" s="7">
+      <c r="P22" s="4">
         <v>0.82</v>
       </c>
-      <c r="Q22" s="7">
+      <c r="Q22" s="4">
         <v>3.72</v>
       </c>
-      <c r="R22" s="7">
+      <c r="R22" s="4">
         <v>1.26</v>
       </c>
-      <c r="S22" s="39">
+      <c r="S22" s="32">
         <f>O22/Q22</f>
         <v>0.65591397849462363</v>
       </c>
     </row>
     <row r="23" spans="2:19" x14ac:dyDescent="0.4">
-      <c r="B23" s="12"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7" t="s">
+      <c r="B23" s="9"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7">
+      <c r="G23" s="4"/>
+      <c r="H23" s="4">
         <v>3</v>
       </c>
-      <c r="I23" s="7">
+      <c r="I23" s="4">
         <v>2.8</v>
       </c>
-      <c r="J23" s="7">
+      <c r="J23" s="4">
         <v>0.95</v>
       </c>
-      <c r="K23" s="7">
+      <c r="K23" s="4">
         <v>6.12</v>
       </c>
-      <c r="L23" s="7">
+      <c r="L23" s="4">
         <v>2.11</v>
       </c>
-      <c r="M23" s="9">
-        <f t="shared" ref="M23:M24" si="5">K23/I23</f>
+      <c r="M23" s="6">
+        <f t="shared" ref="M23:M24" si="6">K23/I23</f>
         <v>2.1857142857142859</v>
       </c>
-      <c r="N23" s="9">
-        <f t="shared" ref="N23:N24" si="6">L23/J23</f>
+      <c r="N23" s="6">
+        <f t="shared" ref="N23:N24" si="7">L23/J23</f>
         <v>2.2210526315789472</v>
       </c>
-      <c r="O23" s="7">
+      <c r="O23" s="4">
         <v>2.44</v>
       </c>
-      <c r="P23" s="7">
+      <c r="P23" s="4">
         <v>0.82</v>
       </c>
-      <c r="Q23" s="7">
+      <c r="Q23" s="4">
         <v>3.72</v>
       </c>
-      <c r="R23" s="7">
+      <c r="R23" s="4">
         <v>1.26</v>
       </c>
-      <c r="S23" s="39">
+      <c r="S23" s="32">
         <f>O23/Q23</f>
         <v>0.65591397849462363</v>
       </c>
     </row>
     <row r="24" spans="2:19" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="15" t="s">
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="H24" s="16">
+      <c r="H24" s="13">
         <v>3</v>
       </c>
-      <c r="I24" s="16">
+      <c r="I24" s="13">
         <v>2.84</v>
       </c>
-      <c r="J24" s="16">
+      <c r="J24" s="13">
         <v>0.95</v>
       </c>
-      <c r="K24" s="16">
+      <c r="K24" s="13">
         <v>6.12</v>
       </c>
-      <c r="L24" s="16">
+      <c r="L24" s="13">
         <v>2.09</v>
       </c>
-      <c r="M24" s="17">
-        <f t="shared" si="5"/>
+      <c r="M24" s="14">
+        <f t="shared" si="6"/>
         <v>2.154929577464789</v>
       </c>
-      <c r="N24" s="17">
-        <f t="shared" si="6"/>
+      <c r="N24" s="14">
+        <f t="shared" si="7"/>
         <v>2.1999999999999997</v>
       </c>
-      <c r="O24" s="16">
+      <c r="O24" s="13">
         <v>2.76</v>
       </c>
-      <c r="P24" s="16">
+      <c r="P24" s="13">
         <v>0.93</v>
       </c>
-      <c r="Q24" s="16">
+      <c r="Q24" s="13">
         <v>3.24</v>
       </c>
-      <c r="R24" s="16">
+      <c r="R24" s="13">
         <v>1.1000000000000001</v>
       </c>
-      <c r="S24" s="45">
+      <c r="S24" s="38">
         <f>O24/Q24</f>
         <v>0.85185185185185175</v>
       </c>
@@ -1854,322 +3422,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="M19:N19"/>
     <mergeCell ref="O19:P19"/>
     <mergeCell ref="Q19:R19"/>
     <mergeCell ref="S19:S20"/>
     <mergeCell ref="L7:M7"/>
     <mergeCell ref="N7:O7"/>
     <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="M19:N19"/>
-  </mergeCells>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E953C177-0DFA-4874-B49C-BF9F6EC2E1F7}">
-  <dimension ref="B3:T11"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
-  <sheetData>
-    <row r="3" spans="2:20" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
-    <row r="4" spans="2:20" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="D4" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E4" s="2"/>
-      <c r="M4" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="N4" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="O4" s="21"/>
-      <c r="P4" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q4" s="21"/>
-      <c r="R4" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="S4" s="22"/>
-    </row>
-    <row r="5" spans="2:20" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F5" t="s">
-        <v>44</v>
-      </c>
-      <c r="G5" t="s">
-        <v>45</v>
-      </c>
-      <c r="H5" t="s">
-        <v>4</v>
-      </c>
-      <c r="I5" t="s">
-        <v>48</v>
-      </c>
-      <c r="J5" t="s">
-        <v>49</v>
-      </c>
-      <c r="K5" t="s">
-        <v>52</v>
-      </c>
-      <c r="L5" t="s">
-        <v>53</v>
-      </c>
-      <c r="M5" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="N5" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="O5" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="P5" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q5" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="R5" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="S5" s="30" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="2:20" x14ac:dyDescent="0.4">
-      <c r="B6" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="F6" s="5">
-        <v>4.99</v>
-      </c>
-      <c r="G6" s="5">
-        <v>1</v>
-      </c>
-      <c r="H6" s="5">
-        <f>1+F6/G6</f>
-        <v>5.99</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="K6" s="5">
-        <v>0</v>
-      </c>
-      <c r="L6" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="M6" s="5">
-        <v>0.6</v>
-      </c>
-      <c r="N6" s="5">
-        <v>0.52</v>
-      </c>
-      <c r="O6" s="5">
-        <v>0.16</v>
-      </c>
-      <c r="P6" s="5">
-        <v>2.64</v>
-      </c>
-      <c r="Q6" s="5">
-        <v>0.9</v>
-      </c>
-      <c r="R6" s="26">
-        <f>P6/N6</f>
-        <v>5.0769230769230766</v>
-      </c>
-      <c r="S6" s="28">
-        <f>Q6/O6</f>
-        <v>5.625</v>
-      </c>
-    </row>
-    <row r="7" spans="2:20" x14ac:dyDescent="0.4">
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7" t="s">
-        <v>6</v>
-      </c>
-      <c r="M7">
-        <v>0.6</v>
-      </c>
-      <c r="P7">
-        <v>12</v>
-      </c>
-      <c r="Q7">
-        <v>12</v>
-      </c>
-      <c r="T7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="2:20" x14ac:dyDescent="0.4">
-      <c r="K8">
-        <v>49.9</v>
-      </c>
-      <c r="L8">
-        <v>49.9</v>
-      </c>
-      <c r="M8">
-        <v>0.6</v>
-      </c>
-      <c r="N8">
-        <v>0.52</v>
-      </c>
-      <c r="O8">
-        <v>0.158</v>
-      </c>
-      <c r="P8">
-        <v>1.24</v>
-      </c>
-      <c r="Q8">
-        <v>0.4</v>
-      </c>
-      <c r="R8" s="46">
-        <f>P8/N8</f>
-        <v>2.3846153846153846</v>
-      </c>
-      <c r="S8" s="47">
-        <f>Q8/O8</f>
-        <v>2.5316455696202533</v>
-      </c>
-    </row>
-    <row r="9" spans="2:20" x14ac:dyDescent="0.4">
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9" t="s">
-        <v>15</v>
-      </c>
-      <c r="M9">
-        <v>0.6</v>
-      </c>
-      <c r="N9">
-        <v>0.52</v>
-      </c>
-      <c r="O9">
-        <v>0.158</v>
-      </c>
-      <c r="P9">
-        <v>2.6</v>
-      </c>
-      <c r="Q9">
-        <v>0.88900000000000001</v>
-      </c>
-      <c r="R9" s="46">
-        <f>P9/N9</f>
-        <v>5</v>
-      </c>
-      <c r="S9" s="47">
-        <f>Q9/O9</f>
-        <v>5.6265822784810124</v>
-      </c>
-    </row>
-    <row r="10" spans="2:20" x14ac:dyDescent="0.4">
-      <c r="J10" t="s">
-        <v>19</v>
-      </c>
-      <c r="M10">
-        <v>0.6</v>
-      </c>
-      <c r="N10">
-        <v>0.52</v>
-      </c>
-      <c r="O10">
-        <v>0.158</v>
-      </c>
-      <c r="P10">
-        <v>2.64</v>
-      </c>
-      <c r="Q10">
-        <v>0.90700000000000003</v>
-      </c>
-      <c r="R10" s="46">
-        <f>P10/N10</f>
-        <v>5.0769230769230766</v>
-      </c>
-      <c r="S10" s="47">
-        <f>Q10/O10</f>
-        <v>5.7405063291139244</v>
-      </c>
-    </row>
-    <row r="11" spans="2:20" x14ac:dyDescent="0.4">
-      <c r="F11" s="5">
-        <v>4.99</v>
-      </c>
-      <c r="G11" s="5">
-        <v>0.80600000000000005</v>
-      </c>
-      <c r="H11" s="6">
-        <f>1+F11/G11</f>
-        <v>7.1910669975186101</v>
-      </c>
-      <c r="M11">
-        <v>0.6</v>
-      </c>
-      <c r="N11">
-        <v>0.52</v>
-      </c>
-      <c r="O11">
-        <v>0.158</v>
-      </c>
-      <c r="P11">
-        <v>2.76</v>
-      </c>
-      <c r="Q11">
-        <v>0.94</v>
-      </c>
-      <c r="R11" s="48">
-        <f>P11/N11</f>
-        <v>5.3076923076923075</v>
-      </c>
-      <c r="S11" s="48">
-        <f>Q11/O11</f>
-        <v>5.9493670886075947</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="R4:S4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>